<commit_message>
Update expected answer in test 5
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test5/QuerySet5.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test5/QuerySet5.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Index</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Expected Answer</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>BUG</t>
   </si>
   <si>
@@ -52,6 +49,12 @@
   </si>
   <si>
     <t>Select v such that Modifies (a, v) pattern a1 (v, _)</t>
+  </si>
+  <si>
+    <t>x,left,right,temp,radius,radius1,quota,iter</t>
+  </si>
+  <si>
+    <t>Get all variables on left hand side of assignment</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,10 +519,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -527,18 +530,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="4"/>
       <c r="G2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>